<commit_message>
Solves expert samurai by brute force
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dean\source\repos\Sudoku\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F320BAED-E4F8-42BD-8B1A-34537B6EA589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9345EFF-90AC-419A-9B4F-67F15284E40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58095" yWindow="-4680" windowWidth="24105" windowHeight="14520" firstSheet="1" activeTab="7" xr2:uid="{1CDF8E94-643E-4348-B7A2-F7C038426B13}"/>
+    <workbookView xWindow="57480" yWindow="-4875" windowWidth="25440" windowHeight="15390" firstSheet="7" activeTab="15" xr2:uid="{1CDF8E94-643E-4348-B7A2-F7C038426B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Samurai (2)" sheetId="7" r:id="rId13"/>
     <sheet name="Samurai (4)" sheetId="9" r:id="rId14"/>
     <sheet name="Samurai (5)" sheetId="11" r:id="rId15"/>
+    <sheet name="Samurai (6)" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4184,6 +4185,745 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50BF317-EB9D-4DFE-B7AA-07171D6521BD}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:U21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="21" width="3.46484375" customWidth="1"/>
+    <col min="22" max="22" width="7.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1" s="34"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24">
+        <v>9</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="23">
+        <v>5</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="23">
+        <v>1</v>
+      </c>
+      <c r="N1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="23">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="24">
+        <v>7</v>
+      </c>
+      <c r="U1" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28">
+        <v>5</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29">
+        <v>4</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28">
+        <v>8</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="29">
+        <v>3</v>
+      </c>
+      <c r="S2" s="27"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31">
+        <v>7</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32">
+        <v>9</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31">
+        <v>2</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31">
+        <v>5</v>
+      </c>
+      <c r="U3" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24">
+        <v>6</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24">
+        <v>2</v>
+      </c>
+      <c r="F4" s="25">
+        <v>5</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24">
+        <v>4</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="25">
+        <v>5</v>
+      </c>
+      <c r="P4" s="23">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25">
+        <v>4</v>
+      </c>
+      <c r="S4" s="23">
+        <v>9</v>
+      </c>
+      <c r="T4" s="24"/>
+      <c r="U4" s="25"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29">
+        <v>6</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="27">
+        <v>8</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
+    </row>
+    <row r="6" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31">
+        <v>3</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="30">
+        <v>1</v>
+      </c>
+      <c r="E6" s="31">
+        <v>4</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31">
+        <v>2</v>
+      </c>
+      <c r="I6" s="32"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="32">
+        <v>9</v>
+      </c>
+      <c r="P6" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32">
+        <v>1</v>
+      </c>
+      <c r="S6" s="30">
+        <v>6</v>
+      </c>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A7" s="23">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24">
+        <v>6</v>
+      </c>
+      <c r="L7" s="25"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24">
+        <v>3</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="24">
+        <v>2</v>
+      </c>
+      <c r="U7" s="25"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28">
+        <v>2</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="27">
+        <v>7</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="27">
+        <v>6</v>
+      </c>
+      <c r="H8" s="28"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="27">
+        <v>4</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29">
+        <v>9</v>
+      </c>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="27">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="29">
+        <v>5</v>
+      </c>
+      <c r="S8" s="27"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="29"/>
+    </row>
+    <row r="9" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32">
+        <v>7</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31">
+        <v>1</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="30">
+        <v>3</v>
+      </c>
+      <c r="H9" s="31">
+        <v>9</v>
+      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="31">
+        <v>6</v>
+      </c>
+      <c r="O9" s="32">
+        <v>8</v>
+      </c>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="32">
+        <v>9</v>
+      </c>
+      <c r="S9" s="30"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="23">
+        <v>8</v>
+      </c>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25">
+        <v>5</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="25">
+        <v>9</v>
+      </c>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28">
+        <v>3</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28">
+        <v>9</v>
+      </c>
+      <c r="L11" s="29"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28">
+        <v>1</v>
+      </c>
+      <c r="O11" s="29"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+    </row>
+    <row r="12" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="30">
+        <v>2</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="30">
+        <v>3</v>
+      </c>
+      <c r="K12" s="31"/>
+      <c r="L12" s="32">
+        <v>6</v>
+      </c>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="23">
+        <v>9</v>
+      </c>
+      <c r="H13" s="24">
+        <v>8</v>
+      </c>
+      <c r="I13" s="25"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="24">
+        <v>5</v>
+      </c>
+      <c r="O13" s="25">
+        <v>7</v>
+      </c>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="23">
+        <v>9</v>
+      </c>
+      <c r="T13" s="24">
+        <v>2</v>
+      </c>
+      <c r="U13" s="25"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="27">
+        <v>1</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28">
+        <v>6</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="27">
+        <v>9</v>
+      </c>
+      <c r="K14" s="33"/>
+      <c r="L14" s="29">
+        <v>1</v>
+      </c>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="29">
+        <v>6</v>
+      </c>
+      <c r="P14" s="27">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="29">
+        <v>9</v>
+      </c>
+      <c r="S14" s="27">
+        <v>3</v>
+      </c>
+      <c r="T14" s="28"/>
+      <c r="U14" s="29"/>
+    </row>
+    <row r="15" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31">
+        <v>6</v>
+      </c>
+      <c r="C15" s="32">
+        <v>5</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31">
+        <v>9</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31">
+        <v>2</v>
+      </c>
+      <c r="I15" s="32"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31">
+        <v>5</v>
+      </c>
+      <c r="L15" s="32"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="32"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24">
+        <v>4</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="23">
+        <v>6</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25">
+        <v>9</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24">
+        <v>1</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="23">
+        <v>3</v>
+      </c>
+      <c r="N16" s="24"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28">
+        <v>8</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28">
+        <v>4</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="29">
+        <v>9</v>
+      </c>
+      <c r="P17" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="29">
+        <v>8</v>
+      </c>
+      <c r="S17" s="27">
+        <v>2</v>
+      </c>
+      <c r="T17" s="28"/>
+      <c r="U17" s="29"/>
+    </row>
+    <row r="18" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31">
+        <v>5</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30">
+        <v>1</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32">
+        <v>2</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31">
+        <v>3</v>
+      </c>
+      <c r="I18" s="32"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="30">
+        <v>2</v>
+      </c>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24">
+        <v>3</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24">
+        <v>7</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="23">
+        <v>1</v>
+      </c>
+      <c r="H19" s="24">
+        <v>6</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="25">
+        <v>2</v>
+      </c>
+      <c r="S19" s="23"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="25"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A20" s="27">
+        <v>8</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28">
+        <v>1</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="29">
+        <v>7</v>
+      </c>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="29">
+        <v>2</v>
+      </c>
+      <c r="P20" s="27">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="29">
+        <v>4</v>
+      </c>
+      <c r="S20" s="27">
+        <v>5</v>
+      </c>
+      <c r="T20" s="28">
+        <v>8</v>
+      </c>
+      <c r="U20" s="29"/>
+    </row>
+    <row r="21" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32">
+        <v>9</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31">
+        <v>1</v>
+      </c>
+      <c r="O21" s="32">
+        <v>5</v>
+      </c>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="30">
+        <v>4</v>
+      </c>
+      <c r="T21" s="31"/>
+      <c r="U21" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4466F0C1-66A8-4FD6-9E56-EBC04A3FD144}">
   <dimension ref="A1:I9"/>
@@ -5189,7 +5929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC428E10-B139-4405-8F12-4489DD7D14B1}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
+    <sheetView zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>